<commit_message>
updated repo_id column with the five first uploaded indicators
</commit_message>
<xml_diff>
--- a/concepts-in-gapminder-indicators.xlsx
+++ b/concepts-in-gapminder-indicators.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-50100" yWindow="-6520" windowWidth="49040" windowHeight="25120" tabRatio="500"/>
+    <workbookView xWindow="-50420" yWindow="-7280" windowWidth="49040" windowHeight="25120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="66">
   <si>
     <t>income_per_person_gdppercapita_ppp_inflation_adjusted</t>
   </si>
@@ -220,6 +220,15 @@
   </si>
   <si>
     <t>pop</t>
+  </si>
+  <si>
+    <t>lex</t>
+  </si>
+  <si>
+    <t>u5mr</t>
+  </si>
+  <si>
+    <t>tfr</t>
   </si>
 </sst>
 </file>
@@ -249,7 +258,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,6 +268,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -275,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -286,6 +301,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -567,16 +584,16 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="35.1640625" customWidth="1"/>
+    <col min="2" max="2" width="39.1640625" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
     <col min="4" max="4" width="15.83203125" customWidth="1"/>
-    <col min="5" max="5" width="28.83203125" customWidth="1"/>
+    <col min="5" max="5" width="35.83203125" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
     <col min="8" max="8" width="20.33203125" customWidth="1"/>
     <col min="9" max="9" width="16.33203125" customWidth="1"/>
@@ -591,7 +608,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>60</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -646,7 +663,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="1" customFormat="1" ht="179" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" s="1" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>61</v>
       </c>
@@ -677,13 +694,13 @@
       <c r="N2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="6" t="s">
         <v>50</v>
       </c>
       <c r="R2" s="1" t="s">
@@ -726,6 +743,9 @@
       </c>
     </row>
     <row r="4" spans="1:18" s="1" customFormat="1" ht="179" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
@@ -758,6 +778,9 @@
       <c r="Q4" s="2"/>
     </row>
     <row r="5" spans="1:18" s="1" customFormat="1" ht="179" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
@@ -790,32 +813,35 @@
       <c r="Q5" s="2"/>
     </row>
     <row r="6" spans="1:18" s="1" customFormat="1" ht="179" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
@@ -823,31 +849,31 @@
     </row>
     <row r="7" spans="1:18" s="1" customFormat="1" ht="179" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>

</xml_diff>